<commit_message>
Modelo de Dados (documentação)
</commit_message>
<xml_diff>
--- a/documentacao/burndownSegundoSprint.xlsx
+++ b/documentacao/burndownSegundoSprint.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TCC\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vinicius Piantoni\TCC\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478C9998-BCDF-4724-B3CF-5FD58FB1EEC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="Restante">OFFSET(Planilha1!$B$12,0,0,1,COUNT(Planilha1!$B$12:$V$12))</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -159,7 +158,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -354,6 +353,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -886,6 +886,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -916,6 +917,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -923,7 +925,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -1020,6 +1021,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1163,7 +1165,10 @@
                   <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1473,6 +1478,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1503,6 +1509,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1510,7 +1517,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -3001,11 +3007,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4025,8 +4031,12 @@
       <c r="B19" s="4">
         <v>12</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -4053,8 +4063,12 @@
       <c r="B20" s="4">
         <v>10</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -4081,8 +4095,12 @@
       <c r="B21" s="4">
         <v>9</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -4109,8 +4127,12 @@
       <c r="B22" s="4">
         <v>14</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -4137,8 +4159,12 @@
       <c r="B23" s="4">
         <v>12</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -4165,8 +4191,12 @@
       <c r="B24" s="4">
         <v>8</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="C24" s="4">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -4193,8 +4223,12 @@
       <c r="B25" s="4">
         <v>11</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2</v>
+      </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -4221,8 +4255,12 @@
       <c r="B26" s="4">
         <v>12</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -4249,8 +4287,12 @@
       <c r="B27" s="4">
         <v>14</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -4277,8 +4319,12 @@
       <c r="B28" s="4">
         <v>18</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
+        <v>3</v>
+      </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -4306,11 +4352,14 @@
         <f>SUM(B19:B28)</f>
         <v>120</v>
       </c>
-      <c r="C29" s="4" t="str">
+      <c r="C29" s="4">
         <f>IF(SUM(C19:C28)&gt;0,B29-SUM(C19:C28),"")</f>
-        <v/>
-      </c>
-      <c r="D29" s="4"/>
+        <v>116</v>
+      </c>
+      <c r="D29" s="4">
+        <f>IF(SUM(D19:D28)&gt;0,C29-SUM(D19:D28),"")</f>
+        <v>109</v>
+      </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -4339,83 +4388,83 @@
         <v>120</v>
       </c>
       <c r="C30" s="4">
-        <f>B30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" ref="C30:V30" si="9">B30-($B$30/COUNTA($C$1:$V$1))</f>
         <v>114</v>
       </c>
       <c r="D30" s="4">
-        <f>C30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>108</v>
       </c>
       <c r="E30" s="4">
-        <f>D30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>102</v>
       </c>
       <c r="F30" s="4">
-        <f>E30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>96</v>
       </c>
       <c r="G30" s="4">
-        <f>F30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
       <c r="H30" s="4">
-        <f>G30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>84</v>
       </c>
       <c r="I30" s="4">
-        <f>H30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>78</v>
       </c>
       <c r="J30" s="4">
-        <f>I30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>72</v>
       </c>
       <c r="K30" s="4">
-        <f>J30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>66</v>
       </c>
       <c r="L30" s="4">
-        <f>K30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="M30" s="4">
-        <f>L30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>54</v>
       </c>
       <c r="N30" s="4">
-        <f>M30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>48</v>
       </c>
       <c r="O30" s="4">
-        <f>N30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>42</v>
       </c>
       <c r="P30" s="4">
-        <f>O30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>36</v>
       </c>
       <c r="Q30" s="4">
-        <f>P30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="R30" s="4">
-        <f>Q30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="S30" s="4">
-        <f>R30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="T30" s="4">
-        <f>S30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="U30" s="4">
-        <f>T30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="V30" s="4">
-        <f>U30-($B$30/COUNTA($C$1:$V$1))</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>